<commit_message>
kafka testcase updated (#7)
Co-authored-by: elanj <elans3.java@gmail.com>
</commit_message>
<xml_diff>
--- a/rest-db-kafka/src/test/resources/event-xls/CreateProduct-Event.xlsx
+++ b/rest-db-kafka/src/test/resources/event-xls/CreateProduct-Event.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\2022\feb-release\microservices-lowcode-testautomation\rest-db-kafka\src\test\resources\event-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B050FFF-CA97-403C-AE6B-84ABF5F515AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3285359B-4AD0-4878-9EB2-C5FFD380C9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductCreated-Event" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>apiservice</t>
   </si>
   <si>
-    <t>http://localhost:8800/product/5</t>
-  </si>
-  <si>
     <t>Validate created product event</t>
   </si>
   <si>
@@ -141,12 +138,15 @@
     <t>productId_,productName_,productDesc_
 i~[productId],Dell Inspiron 3583 15,Laptop Intel Celeron – 128GB SSD – 4GB DDR4 – 1.6GHz - Intel UHD Graphics 610 - Windows 10 Home in S Mode - Inspiron 15 3000 Series</t>
   </si>
+  <si>
+    <t>http://localhost:8800/product/0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -192,6 +192,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -255,12 +261,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,10 +283,12 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
     <cellStyle name="Accent3" xfId="1" builtinId="37"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -499,7 +508,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -583,13 +592,13 @@
         <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -597,11 +606,11 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>5</v>
@@ -624,13 +633,13 @@
         <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -642,10 +651,10 @@
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>

</xml_diff>